<commit_message>
corrected species' name error centroura and ferox
</commit_message>
<xml_diff>
--- a/data/IUCN_DD_FR.xlsx
+++ b/data/IUCN_DD_FR.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,35 +365,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>DD</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>LC</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>NT</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>VU</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>EN</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>CR</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -402,7 +407,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Baltic Sea</t>
         </is>
       </c>
       <c r="B2">
@@ -418,29 +423,32 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Baltic Sea</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -449,132 +457,147 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <v>6</v>
       </c>
+      <c r="I4">
+        <v>53</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Mediterranean Sea</t>
         </is>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="I7">
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -583,128 +606,81 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
+      <c r="I8">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mediterranean Sea</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>4</v>
-      </c>
-      <c r="G9">
-        <v>10</v>
-      </c>
-      <c r="H9">
-        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>World</t>
         </is>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Sweden</t>
-        </is>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>World</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>17</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>15</v>
-      </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-      <c r="G12">
         <v>8</v>
       </c>
-      <c r="H12">
-        <v>60</v>
+      <c r="I10">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated zsl with baltic sea
</commit_message>
<xml_diff>
--- a/data/IUCN_DD_FR.xlsx
+++ b/data/IUCN_DD_FR.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,40 +365,50 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>DD</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>LC</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>NT</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>VU</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>EN</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>CR</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>RE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -407,7 +417,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Baltic Sea</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="B2">
@@ -423,208 +433,250 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Baltic Sea</t>
         </is>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <v>8</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>53</v>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
       <c r="G5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Mediterranean Sea</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
         <v>12</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>7</v>
       </c>
       <c r="G7">
         <v>4</v>
       </c>
       <c r="H7">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I8">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Mediterranean Sea</t>
         </is>
       </c>
       <c r="B9">
@@ -634,52 +686,175 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I9">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>NE Atlantic</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>World</t>
         </is>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="E13">
         <v>17</v>
       </c>
-      <c r="E10">
+      <c r="F13">
         <v>9</v>
       </c>
-      <c r="F10">
+      <c r="G13">
         <v>17</v>
       </c>
-      <c r="G10">
+      <c r="H13">
         <v>9</v>
       </c>
-      <c r="H10">
+      <c r="I13">
         <v>8</v>
       </c>
-      <c r="I10">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>62</v>
       </c>
     </row>

</xml_diff>